<commit_message>
cann add to rightfull fields
</commit_message>
<xml_diff>
--- a/public/templates/upload_tenders.xlsx
+++ b/public/templates/upload_tenders.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp7\htdocs\tenders\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="24000" windowHeight="11010"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="24000" windowHeight="11010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,88 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
-  <si>
-    <t>ICB</t>
-  </si>
-  <si>
-    <t>Self-Funded</t>
-  </si>
-  <si>
-    <t>Kenya , Eastern Africa</t>
-  </si>
-  <si>
-    <t>Plz Refer Document</t>
-  </si>
-  <si>
-    <t>M-KOPA KENYA LIMITED</t>
-  </si>
-  <si>
-    <t>General Procurement Notice for Executing Human-Centered Design Research To Test The Applicability Of Smartphone-Enabled Digital Financial Services For Women</t>
-  </si>
-  <si>
-    <t>African Development Bank (AfDB)</t>
-  </si>
-  <si>
-    <t>Executing Human-Centered Design Research To Test The Applicability Of Smartphone-Enabled Digital Financial Services For Women
-The Principal Objectives Of This Project Are To :
-Design New Gender-Centric Digital Financial Services (Dfs) Innovation For Women Smes In Kenya. The Project Will Assess Factors That Influence Women’S Uptake And Utility Of Mobile Services And Dfs Through Customer Surveys And Focus Group Discussions. Insights From Customer Research Will Inform Product Development To Enhance Financial Literacy And Greater Uptake Of Relevant Dfs.
-The Project Includes The Following Components :
-A. Gender/Hcd Consultancy – Develop Questionnaire And Research Tools For Remote Survey Data Collection And In-Person Focus Group Discussions And Deliver Insights Around Customer Dfs Needs Assessment And Behavioral And Knowledge Perceptions Of Smartphone-Enabled Value-Add Information Services And Dfs.
-B. Software Development Consultancy – Develop Prototype Smartphone Interface And Features Based On Research Findings And User Requirements And Iterate To Deliver Mvp Based On Customer Feedback.</t>
-  </si>
-  <si>
-    <t>Chania Avenue, Off ring-road PO Box 51866-00100 Kilimani, Nairobi Kenya</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tilak Nathwani email address: tilak.nathwani@m-kopa.com telephone number: +44 (0) 7776 690370</t>
-  </si>
-  <si>
-    <t>CENTRAL BANK OF KENYA</t>
-  </si>
-  <si>
-    <t>CBK/ 91 /2021-2022</t>
-  </si>
-  <si>
-    <t>Tenders Are Invited For Provision Of Accommodation And Conference Facilities</t>
-  </si>
-  <si>
-    <t>Tenders Are Invited For Provision Of Accommodation And Conference Facilities For The Central Bank Of Kenya
-Procurement Method: Open Tender
-Submission Method: Written (Physical/Hard Copy)
-Opening Venue: Central Bank Of Kenya Head Office In Nairobi On The Mezzanine Floor Conference Room
-Closing Date: Apr 26, 2022
-Closing Time: 10:00</t>
-  </si>
-  <si>
-    <t>Haile Selassie Avenue P. O. Box 60000 Nairobi Kenya Telephone 2860000 Telex 22324 Fax 310604/340192</t>
-  </si>
-  <si>
-    <t>supplies@centralbank.go.ke</t>
-  </si>
-  <si>
-    <t>MOI UNIVERSITY</t>
-  </si>
-  <si>
-    <t>MU/RFP/15/2021 - 2022</t>
-  </si>
-  <si>
-    <t>Request for Proposal For Provision Of Resource Mobilization For Apple Farming</t>
-  </si>
-  <si>
-    <t>Request For Proposals Are Invited For Provision Of Resource Mobilization For Apple Farming At Moi University Main Campus
-Submission Method: Written (Physical/Hard Copy)
-Opening Venue: Moi University Main Campus, Kesses Administration &amp; Senate Building Boardroom
-Closing Date: Apr 28, 2022
-Closing Time: 11:00
-Tender Document For Hard Copy Only Kes. Non Refundable 1,000.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Office of the Deputy Vice Chancellor Finance P. O. Box 3900 Eldoret-30100 Kenya. Tel: (053) 43321 Ext. 2122</t>
-  </si>
-  <si>
-    <t>dvc_f@mu.ac.ke, Supplies@mu.ac.ke</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>LINKS</t>
   </si>
@@ -141,9 +60,6 @@
   </si>
   <si>
     <t>PURCHASING AUTHORITY</t>
-  </si>
-  <si>
-    <t>2021/S 158-413043</t>
   </si>
   <si>
     <t>TENDER BRIEF</t>
@@ -156,8 +72,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -185,9 +109,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,175 +394,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" customWidth="1"/>
-    <col min="10" max="10" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="98.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="91.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" customWidth="1"/>
     <col min="13" max="13" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="1">
-        <v>44789</v>
-      </c>
-      <c r="K2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="1">
-        <v>44677</v>
-      </c>
-      <c r="K3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="1">
-        <v>44679</v>
-      </c>
-      <c r="K4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>